<commit_message>
rebasing repo based on wealth tax code and data
</commit_message>
<xml_diff>
--- a/Data/Calibration/ConsumptionParameters/CEX_ConsumptionCategories_byLevel.xlsx
+++ b/Data/Calibration/ConsumptionParameters/CEX_ConsumptionCategories_byLevel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14920" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="14920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook" sheetId="1" r:id="rId1"/>
@@ -4117,9 +4117,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1359"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A344" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C355" sqref="C355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -62699,13 +62699,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">

</xml_diff>